<commit_message>
keeping data away from public access...
</commit_message>
<xml_diff>
--- a/DATAFRAME (SOLAR_ECLIPSE_SAFARI) [ZIPCODE].xlsx
+++ b/DATAFRAME (SOLAR_ECLIPSE_SAFARI) [ZIPCODE].xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d9d79303ce864b82/Desktop/OBSCURATION ALGORITHM/OBSCURATION-TOTALITY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{6A64416F-9596-4AD3-A392-54F0CBCA0C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F50371E-BEDA-44DF-9473-71DCB2E8C788}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{6A64416F-9596-4AD3-A392-54F0CBCA0C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A253388-88F8-4280-831C-274BF89D9569}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{FE200377-E352-4AB1-8995-A86B899C16DE}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{FE200377-E352-4AB1-8995-A86B899C16DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1135,6 +1135,10 @@
 </file>
 
 <file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1437,8 +1441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15213D02-E120-48E9-92FD-904DE9D02A99}">
   <dimension ref="A1:H663"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A633" workbookViewId="0">
-      <selection activeCell="A665" sqref="A665"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>